<commit_message>
finished compare_gsea.py tests. intergrating existing code to main branch
</commit_message>
<xml_diff>
--- a/pipeline/Outputs/NGSEA/Summary/H_sapiens/Decoy/alpha_0.1/Decoy_Summary_H_sapiens_alpha_0.1.xlsx
+++ b/pipeline/Outputs/NGSEA/Summary/H_sapiens/Decoy/alpha_0.1/Decoy_Summary_H_sapiens_alpha_0.1.xlsx
@@ -14,12 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
   <si>
     <t>Method</t>
   </si>
   <si>
     <t>Average Significant Percentage</t>
+  </si>
+  <si>
+    <t>H_sapiens</t>
   </si>
   <si>
     <t>ABS_PROP</t>
@@ -389,50 +398,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>0.1736111111111111</v>
+        <v>0.1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>0.1362397820163488</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>0.03360215053763441</v>
+        <v>0.1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>0.04541326067211626</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.04607720043783401</v>
+        <v>0.1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>0.04541326067211626</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>0.02170138888888888</v>
+        <v>0.1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>0.01135331516802906</v>
       </c>
     </row>
   </sheetData>

</xml_diff>